<commit_message>
D214 part 2 Update
</commit_message>
<xml_diff>
--- a/D214/Part 2/Pokemon TCG Sealed Prices.xlsx
+++ b/D214/Part 2/Pokemon TCG Sealed Prices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin .LAPTOP-VCUUDDEB\Documents\GitHub\WGU\D214\Part 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9364116-43E6-4A43-8562-AF54ADC5A88A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8B302E-9952-43F9-90BD-64255AC5CD3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4980" yWindow="2955" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,10 +1279,10 @@
         <v>41</v>
       </c>
       <c r="C40" s="2">
+        <v>7.65</v>
+      </c>
+      <c r="D40" s="2">
         <v>359.36</v>
-      </c>
-      <c r="D40" s="2">
-        <v>7.65</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>